<commit_message>
added several supplemental figures/tables
</commit_message>
<xml_diff>
--- a/4_and_5_Binding_Correlations_Figure_Cooptimal/p1_binding_with_ngs_scores.xlsx
+++ b/4_and_5_Binding_Correlations_Figure_Cooptimal/p1_binding_with_ngs_scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -503,10 +503,10 @@
         <v>0.851331573</v>
       </c>
       <c r="D2" t="n">
-        <v>19.54808110716422</v>
+        <v>18.70835811617782</v>
       </c>
       <c r="E2" t="n">
-        <v>2.394884232768992</v>
+        <v>2.394884232768993</v>
       </c>
       <c r="F2" t="n">
         <v>4.081299485756264e-05</v>
@@ -515,10 +515,10 @@
         <v>0.4086221723366428</v>
       </c>
       <c r="H2" t="n">
-        <v>18.70835811617782</v>
+        <v>16.61188720856606</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2984133251572312</v>
+        <v>0.2984133251572303</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -536,10 +536,10 @@
         <v>1.081845563</v>
       </c>
       <c r="D3" t="n">
-        <v>21.17384294955221</v>
+        <v>21.78781819507843</v>
       </c>
       <c r="E3" t="n">
-        <v>3.794802146959261</v>
+        <v>3.794802146959263</v>
       </c>
       <c r="F3" t="n">
         <v>1.997231663242427e-05</v>
@@ -548,10 +548,10 @@
         <v>0.02529353278513709</v>
       </c>
       <c r="H3" t="n">
-        <v>21.78781819507843</v>
+        <v>18.56074126420972</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5677252160905624</v>
+        <v>0.5677252160905606</v>
       </c>
       <c r="J3" t="n">
         <v>4.447331308627237e-05</v>
@@ -573,10 +573,10 @@
         <v>0.813500938</v>
       </c>
       <c r="D4" t="n">
-        <v>22.15848633544546</v>
+        <v>21.21466642386854</v>
       </c>
       <c r="E4" t="n">
-        <v>4.080868320297947</v>
+        <v>4.080868320297949</v>
       </c>
       <c r="F4" t="n">
         <v>1.128870070528329e-05</v>
@@ -585,10 +585,10 @@
         <v>-1.821675447085151</v>
       </c>
       <c r="H4" t="n">
-        <v>21.21466642386854</v>
+        <v>17.33500891643433</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2012108128637409</v>
+        <v>0.2012108128637404</v>
       </c>
       <c r="J4" t="n">
         <v>0.0002165148137094839</v>
@@ -610,10 +610,10 @@
         <v>0.820071338</v>
       </c>
       <c r="D5" t="n">
-        <v>21.42596258786709</v>
+        <v>20.93574573440618</v>
       </c>
       <c r="E5" t="n">
-        <v>3.210347172685363</v>
+        <v>3.210347172685364</v>
       </c>
       <c r="F5" t="n">
         <v>7.381073538069841e-05</v>
@@ -622,10 +622,10 @@
         <v>0.8638167980874695</v>
       </c>
       <c r="H5" t="n">
-        <v>20.93574573440617</v>
+        <v>18.22564475672517</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5002461950043611</v>
+        <v>0.5002461950043608</v>
       </c>
       <c r="J5" t="n">
         <v>0.0001275681875369392</v>
@@ -647,7 +647,7 @@
         <v>0.826149154</v>
       </c>
       <c r="D6" t="n">
-        <v>13.73490213670492</v>
+        <v>14.03055252409274</v>
       </c>
       <c r="E6" t="n">
         <v>-1.401431320986156</v>
@@ -659,10 +659,10 @@
         <v>-0.1763403283845134</v>
       </c>
       <c r="H6" t="n">
-        <v>14.03055252409274</v>
+        <v>15.62993622491712</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1979523798382273</v>
+        <v>0.1979523798382264</v>
       </c>
       <c r="J6" t="n">
         <v>3.628086067564325e-05</v>
@@ -684,10 +684,10 @@
         <v>0.714095195</v>
       </c>
       <c r="D7" t="n">
-        <v>20.00653708191021</v>
+        <v>20.25757979524642</v>
       </c>
       <c r="E7" t="n">
-        <v>2.877247872629217</v>
+        <v>2.87724787262922</v>
       </c>
       <c r="F7" t="n">
         <v>4.341807963570494e-05</v>
@@ -696,10 +696,10 @@
         <v>0.59304674347407</v>
       </c>
       <c r="H7" t="n">
-        <v>20.25757979524642</v>
+        <v>17.89301979498221</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5126878723650006</v>
+        <v>0.512687872365001</v>
       </c>
       <c r="J7" t="n">
         <v>5.266576549690149e-05</v>
@@ -721,7 +721,7 @@
         <v>0.813367036</v>
       </c>
       <c r="D8" t="n">
-        <v>16.8264599432395</v>
+        <v>16.28660367971138</v>
       </c>
       <c r="E8" t="n">
         <v>1.65304917474928</v>
@@ -733,7 +733,7 @@
         <v>-1.176340328384514</v>
       </c>
       <c r="H8" t="n">
-        <v>16.28660367971138</v>
+        <v>15.28955857419547</v>
       </c>
       <c r="I8" t="n">
         <v>0.6560040692333706</v>
@@ -758,10 +758,10 @@
         <v>0.6370990399999999</v>
       </c>
       <c r="D9" t="n">
-        <v>10.46065084207565</v>
+        <v>10.13251572283791</v>
       </c>
       <c r="E9" t="n">
-        <v>-5.503575924106497</v>
+        <v>-5.503575924106495</v>
       </c>
       <c r="F9" t="n">
         <v>1.128870070528329e-05</v>
@@ -770,10 +770,10 @@
         <v>0.2021712948692164</v>
       </c>
       <c r="H9" t="n">
-        <v>10.13251572283791</v>
+        <v>15.07107894917308</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.5650126977713248</v>
+        <v>-0.5650126977713252</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -791,10 +791,10 @@
         <v>1.066888875</v>
       </c>
       <c r="D10" t="n">
-        <v>14.86870200254763</v>
+        <v>14.6118160766635</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.7511575072227319</v>
+        <v>-0.7511575072227321</v>
       </c>
       <c r="F10" t="n">
         <v>1.649887026156788e-05</v>
@@ -803,10 +803,10 @@
         <v>0.1971180671429311</v>
       </c>
       <c r="H10" t="n">
-        <v>14.6118160766635</v>
+        <v>15.90878608759149</v>
       </c>
       <c r="I10" t="n">
-        <v>0.545812503705265</v>
+        <v>0.5458125037052646</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -824,10 +824,10 @@
         <v>0.708621437</v>
       </c>
       <c r="D11" t="n">
-        <v>21.77032912282001</v>
+        <v>22.77725557143994</v>
       </c>
       <c r="E11" t="n">
-        <v>4.494211496700021</v>
+        <v>4.494211496700024</v>
       </c>
       <c r="F11" t="n">
         <v>9.551977519855088e-05</v>
@@ -836,10 +836,10 @@
         <v>0.0001573269812852929</v>
       </c>
       <c r="H11" t="n">
-        <v>22.77725557143994</v>
+        <v>18.55104612863017</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2680020538902421</v>
+        <v>0.2680020538902441</v>
       </c>
       <c r="J11" t="n">
         <v>0.002433158365956849</v>
@@ -861,7 +861,7 @@
         <v>0.765334781</v>
       </c>
       <c r="D12" t="n">
-        <v>22.21927076566983</v>
+        <v>22.81044396872054</v>
       </c>
       <c r="E12" t="n">
         <v>4.546661955161667</v>
@@ -873,10 +873,10 @@
         <v>-0.3283434218295631</v>
       </c>
       <c r="H12" t="n">
-        <v>22.81044396872054</v>
+        <v>18.74742774369592</v>
       </c>
       <c r="I12" t="n">
-        <v>0.483645730137048</v>
+        <v>0.4836457301370458</v>
       </c>
       <c r="J12" t="n">
         <v>0.0001299088882256903</v>
@@ -898,7 +898,7 @@
         <v>0.690410973</v>
       </c>
       <c r="D13" t="n">
-        <v>20.79674327151347</v>
+        <v>20.45184264837387</v>
       </c>
       <c r="E13" t="n">
         <v>3.471031157598676</v>
@@ -910,10 +910,10 @@
         <v>-0.7840229056057529</v>
       </c>
       <c r="H13" t="n">
-        <v>20.45184264837386</v>
+        <v>17.42187231657475</v>
       </c>
       <c r="I13" t="n">
-        <v>0.441060825799563</v>
+        <v>0.4410608257995616</v>
       </c>
       <c r="J13" t="n">
         <v>5.851751721877944e-05</v>
@@ -935,18 +935,18 @@
         <v>0.409272856</v>
       </c>
       <c r="D14" t="n">
-        <v>12.72167705188882</v>
+        <v>12.22179047109426</v>
       </c>
       <c r="E14" t="n">
-        <v>-4.272327153196747</v>
+        <v>-4.272327153196745</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>12.22179047109426</v>
+        <v>15.4042377241739</v>
       </c>
       <c r="I14" t="n">
-        <v>-1.089879900117106</v>
+        <v>-1.089879900117107</v>
       </c>
       <c r="J14" t="n">
         <v>1.170350344375589e-06</v>
@@ -968,10 +968,10 @@
         <v>0.662897818</v>
       </c>
       <c r="D15" t="n">
-        <v>21.03031413548556</v>
+        <v>21.15629313688745</v>
       </c>
       <c r="E15" t="n">
-        <v>2.833080809257744</v>
+        <v>2.833080809257746</v>
       </c>
       <c r="F15" t="n">
         <v>8.596779767869579e-05</v>
@@ -980,10 +980,10 @@
         <v>0.1799977972886803</v>
       </c>
       <c r="H15" t="n">
-        <v>21.15629313688745</v>
+        <v>18.68700455831132</v>
       </c>
       <c r="I15" t="n">
-        <v>0.3637922306816104</v>
+        <v>0.3637922306816095</v>
       </c>
       <c r="J15" t="n">
         <v>0.000375682460544564</v>
@@ -1005,10 +1005,10 @@
         <v>1.06150343</v>
       </c>
       <c r="D16" t="n">
-        <v>18.31895102282039</v>
+        <v>18.46045835614044</v>
       </c>
       <c r="E16" t="n">
-        <v>3.256523330529515</v>
+        <v>3.256523330529514</v>
       </c>
       <c r="F16" t="n">
         <v>7.81525433442689e-06</v>
@@ -1017,10 +1017,10 @@
         <v>1.578547173778955</v>
       </c>
       <c r="H16" t="n">
-        <v>18.46045835614044</v>
+        <v>15.99231275138862</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7883777257776921</v>
+        <v>0.7883777257776909</v>
       </c>
       <c r="J16" t="n">
         <v>4.447331308627237e-05</v>
@@ -1042,10 +1042,10 @@
         <v>0.988211668</v>
       </c>
       <c r="D17" t="n">
-        <v>18.68304851605035</v>
+        <v>18.83640741177098</v>
       </c>
       <c r="E17" t="n">
-        <v>2.027115801488067</v>
+        <v>2.027115801488069</v>
       </c>
       <c r="F17" t="n">
         <v>2.257740141056657e-05</v>
@@ -1054,10 +1054,10 @@
         <v>-0.4759006102434212</v>
       </c>
       <c r="H17" t="n">
-        <v>18.83640741177098</v>
+        <v>17.26619296836839</v>
       </c>
       <c r="I17" t="n">
-        <v>0.4569013580854797</v>
+        <v>0.4569013580854804</v>
       </c>
       <c r="J17" t="n">
         <v>8.42652247950424e-05</v>
@@ -1079,10 +1079,10 @@
         <v>0.75540566</v>
       </c>
       <c r="D18" t="n">
-        <v>22.0242603823666</v>
+        <v>21.76884348995441</v>
       </c>
       <c r="E18" t="n">
-        <v>3.452233419874556</v>
+        <v>3.452233419874557</v>
       </c>
       <c r="F18" t="n">
         <v>2.170903981785247e-05</v>
@@ -1091,10 +1091,10 @@
         <v>-0.7548765599462365</v>
       </c>
       <c r="H18" t="n">
-        <v>21.76884348995441</v>
+        <v>18.36869430832971</v>
       </c>
       <c r="I18" t="n">
-        <v>0.05208423824985875</v>
+        <v>0.05208423824985831</v>
       </c>
       <c r="J18" t="n">
         <v>0.0001989595585438501</v>
@@ -1116,10 +1116,10 @@
         <v>0.921320522</v>
       </c>
       <c r="D19" t="n">
-        <v>15.79055053882829</v>
+        <v>16.84457784873161</v>
       </c>
       <c r="E19" t="n">
-        <v>0.09077658679286293</v>
+        <v>0.0907765867928636</v>
       </c>
       <c r="F19" t="n">
         <v>1.476214707613968e-05</v>
@@ -1128,10 +1128,10 @@
         <v>-0.5039149864130179</v>
       </c>
       <c r="H19" t="n">
-        <v>16.84457784873161</v>
+        <v>17.09805467329123</v>
       </c>
       <c r="I19" t="n">
-        <v>0.3442534113524899</v>
+        <v>0.3442534113524888</v>
       </c>
       <c r="J19" t="n">
         <v>4.798436411939914e-05</v>
@@ -1153,10 +1153,10 @@
         <v>0.707709429</v>
       </c>
       <c r="D20" t="n">
-        <v>18.05335117495989</v>
+        <v>16.73062730649282</v>
       </c>
       <c r="E20" t="n">
-        <v>1.077882637318506</v>
+        <v>1.077882637318507</v>
       </c>
       <c r="F20" t="n">
         <v>1.128870070528329e-05</v>
@@ -1165,10 +1165,10 @@
         <v>1.301706968420131</v>
       </c>
       <c r="H20" t="n">
-        <v>16.73062730649282</v>
+        <v>16.10957976720388</v>
       </c>
       <c r="I20" t="n">
-        <v>0.4568350980295597</v>
+        <v>0.4568350980295606</v>
       </c>
       <c r="J20" t="n">
         <v>2.691805792063854e-05</v>
@@ -1190,10 +1190,10 @@
         <v>0.683507395</v>
       </c>
       <c r="D21" t="n">
-        <v>21.07854205360563</v>
+        <v>21.75321918691505</v>
       </c>
       <c r="E21" t="n">
-        <v>3.068422673434701</v>
+        <v>3.068422673434702</v>
       </c>
       <c r="F21" t="n">
         <v>5.904858830455872e-05</v>
@@ -1202,10 +1202,10 @@
         <v>0.1210455822400574</v>
       </c>
       <c r="H21" t="n">
-        <v>21.75321918691505</v>
+        <v>19.02011810422116</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3353215907408085</v>
+        <v>0.3353215907408094</v>
       </c>
       <c r="J21" t="n">
         <v>0.0001884264054444698</v>
@@ -1227,10 +1227,10 @@
         <v>0.416625214</v>
       </c>
       <c r="D22" t="n">
-        <v>20.30623062806979</v>
+        <v>19.74374860627168</v>
       </c>
       <c r="E22" t="n">
-        <v>2.261781416769969</v>
+        <v>2.26178141676997</v>
       </c>
       <c r="F22" t="n">
         <v>0.000149358193946825</v>
@@ -1239,10 +1239,10 @@
         <v>1.425495990901039</v>
       </c>
       <c r="H22" t="n">
-        <v>19.74374860627168</v>
+        <v>17.79421490741208</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3122477179103689</v>
+        <v>0.312247717910368</v>
       </c>
       <c r="J22" t="n">
         <v>0.0003721714095114373</v>
@@ -1264,7 +1264,7 @@
         <v>0.716210251</v>
       </c>
       <c r="D23" t="n">
-        <v>21.85839844179231</v>
+        <v>21.55298493546261</v>
       </c>
       <c r="E23" t="n">
         <v>4.222963177703192</v>
@@ -1276,10 +1276,10 @@
         <v>-0.6963473872648998</v>
       </c>
       <c r="H23" t="n">
-        <v>21.55298493546261</v>
+        <v>17.82007041072784</v>
       </c>
       <c r="I23" t="n">
-        <v>0.4900486529684225</v>
+        <v>0.4900486529684207</v>
       </c>
       <c r="J23" t="n">
         <v>0.0003522754536570522</v>
@@ -1301,10 +1301,10 @@
         <v>0.806437311</v>
       </c>
       <c r="D24" t="n">
-        <v>16.69705575177346</v>
+        <v>17.69860305879524</v>
       </c>
       <c r="E24" t="n">
-        <v>1.799156617467512</v>
+        <v>1.799156617467514</v>
       </c>
       <c r="F24" t="n">
         <v>5.904858830455872e-05</v>
@@ -1313,10 +1313,10 @@
         <v>1.248157500143397</v>
       </c>
       <c r="H24" t="n">
-        <v>17.69860305879524</v>
+        <v>16.16013181305845</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2606853717307188</v>
+        <v>0.26068537173072</v>
       </c>
       <c r="J24" t="n">
         <v>3.394015998689207e-05</v>
@@ -1338,10 +1338,10 @@
         <v>1.006067178</v>
       </c>
       <c r="D25" t="n">
-        <v>23.68727836651708</v>
+        <v>23.93557158630663</v>
       </c>
       <c r="E25" t="n">
-        <v>5.02905505054258</v>
+        <v>5.029055050542582</v>
       </c>
       <c r="F25" t="n">
         <v>5.123333397013183e-05</v>
@@ -1350,10 +1350,10 @@
         <v>-0.01251552647861886</v>
       </c>
       <c r="H25" t="n">
-        <v>23.93557158630663</v>
+        <v>19.50912115187695</v>
       </c>
       <c r="I25" t="n">
-        <v>0.6026046161129015</v>
+        <v>0.6026046161129013</v>
       </c>
       <c r="J25" t="n">
         <v>0.0006097525294196818</v>
@@ -1375,10 +1375,10 @@
         <v>0.6299327</v>
       </c>
       <c r="D26" t="n">
-        <v>13.631368481136</v>
+        <v>13.1926505795087</v>
       </c>
       <c r="E26" t="n">
-        <v>-2.250099503520515</v>
+        <v>-2.250099503520514</v>
       </c>
       <c r="F26" t="n">
         <v>1.823559344699608e-05</v>
@@ -1387,10 +1387,10 @@
         <v>1.100499876974311</v>
       </c>
       <c r="H26" t="n">
-        <v>13.19265057950871</v>
+        <v>15.49976509713668</v>
       </c>
       <c r="I26" t="n">
-        <v>0.05701501410745946</v>
+        <v>0.05701501410746013</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -1408,10 +1408,10 @@
         <v>0.321888143</v>
       </c>
       <c r="D27" t="n">
-        <v>19.38339820285062</v>
+        <v>20.45247125591332</v>
       </c>
       <c r="E27" t="n">
-        <v>2.08865453874742</v>
+        <v>2.088654538747423</v>
       </c>
       <c r="F27" t="n">
         <v>5.036497237741774e-05</v>
@@ -1420,10 +1420,10 @@
         <v>1.31240685707734</v>
       </c>
       <c r="H27" t="n">
-        <v>20.45247125591332</v>
+        <v>18.58144749615976</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2176307789938619</v>
+        <v>0.217630778993863</v>
       </c>
       <c r="J27" t="n">
         <v>1.404420413250707e-05</v>
@@ -1445,18 +1445,18 @@
         <v>0.385127027</v>
       </c>
       <c r="D28" t="n">
-        <v>10.40245617225346</v>
+        <v>9.444197296833567</v>
       </c>
       <c r="E28" t="n">
-        <v>-4.22434498969676</v>
+        <v>-4.224344989696759</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>9.444197296833567</v>
+        <v>12.24625818749493</v>
       </c>
       <c r="I28" t="n">
-        <v>-1.4222840990354</v>
+        <v>-1.422284099035399</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
@@ -1474,7 +1474,7 @@
         <v>0.5791673389999999</v>
       </c>
       <c r="D29" t="n">
-        <v>18.0484763540451</v>
+        <v>18.50946756792049</v>
       </c>
       <c r="E29" t="n">
         <v>2.664548509501821</v>
@@ -1486,10 +1486,10 @@
         <v>-2.498268423271876</v>
       </c>
       <c r="H29" t="n">
-        <v>18.50946756792049</v>
+        <v>16.11308818455639</v>
       </c>
       <c r="I29" t="n">
-        <v>0.268169126137721</v>
+        <v>0.2681691261377193</v>
       </c>
       <c r="J29" t="n">
         <v>4.447331308627237e-05</v>
@@ -1511,10 +1511,10 @@
         <v>0.60425626</v>
       </c>
       <c r="D30" t="n">
-        <v>19.5541396903337</v>
+        <v>20.14911725371923</v>
       </c>
       <c r="E30" t="n">
-        <v>2.513815827699125</v>
+        <v>2.513815827699128</v>
       </c>
       <c r="F30" t="n">
         <v>0.0001163604534236893</v>
@@ -1523,10 +1523,10 @@
         <v>0.3148400260160258</v>
       </c>
       <c r="H30" t="n">
-        <v>20.14911725371922</v>
+        <v>17.88479765161451</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2494962255944102</v>
+        <v>0.2494962255944115</v>
       </c>
       <c r="J30" t="n">
         <v>0.000250454973696376</v>
@@ -1548,10 +1548,10 @@
         <v>0.525406183</v>
       </c>
       <c r="D31" t="n">
-        <v>18.32299702577963</v>
+        <v>16.47611816641983</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8630997574262123</v>
+        <v>0.8630997574262131</v>
       </c>
       <c r="F31" t="n">
         <v>8.683615927140989e-06</v>
@@ -1560,10 +1560,10 @@
         <v>-0.07680465483359888</v>
       </c>
       <c r="H31" t="n">
-        <v>16.47611816641982</v>
+        <v>15.68171524598895</v>
       </c>
       <c r="I31" t="n">
-        <v>0.06869683699533602</v>
+        <v>0.06869683699533402</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
@@ -1581,10 +1581,10 @@
         <v>0.60585142</v>
       </c>
       <c r="D32" t="n">
-        <v>5.303741207804705</v>
+        <v>4.163539394345281</v>
       </c>
       <c r="E32" t="n">
-        <v>-9.136259922448689</v>
+        <v>-9.136259922448684</v>
       </c>
       <c r="F32" t="n">
         <v>4.341807963570494e-06</v>
@@ -1593,7 +1593,7 @@
         <v>-2.313843852134448</v>
       </c>
       <c r="H32" t="n">
-        <v>4.16353939434528</v>
+        <v>12.94094694019077</v>
       </c>
       <c r="I32" t="n">
         <v>-0.3588523766031944</v>
@@ -1614,10 +1614,10 @@
         <v>0.796144601</v>
       </c>
       <c r="D33" t="n">
-        <v>6.656617993771174</v>
+        <v>6.700651309341816</v>
       </c>
       <c r="E33" t="n">
-        <v>-5.965871328215025</v>
+        <v>-5.965871328215023</v>
       </c>
       <c r="F33" t="n">
         <v>8.683615927140989e-07</v>
@@ -1626,10 +1626,10 @@
         <v>-2.398732749720961</v>
       </c>
       <c r="H33" t="n">
-        <v>6.700651309341817</v>
+        <v>13.09151700379999</v>
       </c>
       <c r="I33" t="n">
-        <v>0.4249943662431539</v>
+        <v>0.4249943662431541</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
@@ -1647,10 +1647,10 @@
         <v>0.437966628</v>
       </c>
       <c r="D34" t="n">
-        <v>15.16403451389547</v>
+        <v>15.46849954260049</v>
       </c>
       <c r="E34" t="n">
-        <v>-1.904601005127271</v>
+        <v>-1.904601005127268</v>
       </c>
       <c r="F34" t="n">
         <v>1.736723185428198e-06</v>
@@ -1659,10 +1659,10 @@
         <v>-2.291817545804449</v>
       </c>
       <c r="H34" t="n">
-        <v>15.46849954260049</v>
+        <v>16.5400321226507</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.833068425077054</v>
+        <v>-0.8330684250770529</v>
       </c>
       <c r="J34" t="n">
         <v>1.170350344375589e-06</v>
@@ -1684,7 +1684,7 @@
         <v>0.499175969</v>
       </c>
       <c r="D35" t="n">
-        <v>1.227007947739333</v>
+        <v>1.290029740081234</v>
       </c>
       <c r="E35" t="n">
         <v>-10.2155807850813</v>
@@ -1692,10 +1692,10 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>1.290029740081233</v>
+        <v>10.23941986922571</v>
       </c>
       <c r="I35" t="n">
-        <v>-1.266190655936819</v>
+        <v>-1.266190655936818</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
@@ -1713,7 +1713,7 @@
         <v>0.6851471689999999</v>
       </c>
       <c r="D36" t="n">
-        <v>7.275415450639053</v>
+        <v>8.869424641777156</v>
       </c>
       <c r="E36" t="n">
         <v>-5.118862888969086</v>
@@ -1725,10 +1725,10 @@
         <v>-1.176340328384514</v>
       </c>
       <c r="H36" t="n">
-        <v>8.869424641777155</v>
+        <v>14.38678012115603</v>
       </c>
       <c r="I36" t="n">
-        <v>0.3984925904097922</v>
+        <v>0.3984925904097918</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
@@ -1746,18 +1746,18 @@
         <v>0.751910166</v>
       </c>
       <c r="D37" t="n">
-        <v>2.007364699792368</v>
+        <v>-0.2179045357821263</v>
       </c>
       <c r="E37" t="n">
-        <v>-12.03998891047273</v>
+        <v>-12.03998891047272</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
-        <v>-0.2179045357821257</v>
+        <v>11.66973432145659</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.1523500532340003</v>
+        <v>-0.1523500532340007</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
@@ -1775,10 +1775,10 @@
         <v>0.716273554</v>
       </c>
       <c r="D38" t="n">
-        <v>19.51135653343786</v>
+        <v>20.40555419301792</v>
       </c>
       <c r="E38" t="n">
-        <v>3.737216478130605</v>
+        <v>3.737216478130606</v>
       </c>
       <c r="F38" t="n">
         <v>8.683615927140989e-06</v>
@@ -1787,10 +1787,10 @@
         <v>-0.1763403283845134</v>
       </c>
       <c r="H38" t="n">
-        <v>20.40555419301792</v>
+        <v>17.00934257144948</v>
       </c>
       <c r="I38" t="n">
-        <v>0.3410048565621726</v>
+        <v>0.3410048565621724</v>
       </c>
       <c r="J38" t="n">
         <v>7.607277238441328e-05</v>
@@ -1812,7 +1812,7 @@
         <v>0.656229738</v>
       </c>
       <c r="D39" t="n">
-        <v>7.419264063574577</v>
+        <v>5.457098949465291</v>
       </c>
       <c r="E39" t="n">
         <v>-7.610506153323709</v>
@@ -1824,10 +1824,10 @@
         <v>-0.03883680463457864</v>
       </c>
       <c r="H39" t="n">
-        <v>5.457098949465292</v>
+        <v>13.00643176527852</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.06117333751047882</v>
+        <v>-0.06117333751047993</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
@@ -1845,7 +1845,7 @@
         <v>0.452419879</v>
       </c>
       <c r="D40" t="n">
-        <v>14.33795750158455</v>
+        <v>13.50545764681694</v>
       </c>
       <c r="E40" t="n">
         <v>-2.282902890863729</v>
@@ -1853,10 +1853,10 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>13.50545764681694</v>
+        <v>15.43035728033293</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.3580032573477367</v>
+        <v>-0.3580032573477372</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
@@ -1874,7 +1874,7 @@
         <v>0.722249816</v>
       </c>
       <c r="D41" t="n">
-        <v>2.773981780942944</v>
+        <v>0.4326074580196289</v>
       </c>
       <c r="E41" t="n">
         <v>-11.89321567174351</v>
@@ -1886,10 +1886,10 @@
         <v>2.671656578170437</v>
       </c>
       <c r="H41" t="n">
-        <v>0.432607458019628</v>
+        <v>11.7810266597183</v>
       </c>
       <c r="I41" t="n">
-        <v>-0.5447964700448389</v>
+        <v>-0.5447964700448378</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
@@ -1907,7 +1907,7 @@
         <v>0.30247576</v>
       </c>
       <c r="D42" t="n">
-        <v>2.698236300408522</v>
+        <v>2.189784869515821</v>
       </c>
       <c r="E42" t="n">
         <v>-11.40241170612937</v>
@@ -1915,7 +1915,7 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>2.18978486951582</v>
+        <v>11.62918995108879</v>
       </c>
       <c r="I42" t="n">
         <v>-1.963006624556405</v>
@@ -1936,7 +1936,7 @@
         <v>0.663863557</v>
       </c>
       <c r="D43" t="n">
-        <v>9.177878907875368</v>
+        <v>9.444840389407188</v>
       </c>
       <c r="E43" t="n">
         <v>-4.825273439396264</v>
@@ -1948,10 +1948,10 @@
         <v>0.5461256960865778</v>
       </c>
       <c r="H43" t="n">
-        <v>9.44484038940719</v>
+        <v>14.35836068480814</v>
       </c>
       <c r="I43" t="n">
-        <v>0.08824685600468996</v>
+        <v>0.08824685600468973</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
@@ -1969,7 +1969,7 @@
         <v>0.422166471</v>
       </c>
       <c r="D44" t="n">
-        <v>10.45750247300143</v>
+        <v>10.8966410157768</v>
       </c>
       <c r="E44" t="n">
         <v>-3.922149984252447</v>
@@ -1981,10 +1981,10 @@
         <v>0.4086221723366428</v>
       </c>
       <c r="H44" t="n">
-        <v>10.8966410157768</v>
+        <v>14.20980002551697</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.6089909745122799</v>
+        <v>-0.6089909745122815</v>
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
@@ -2002,18 +2002,18 @@
         <v>0.5715419269999999</v>
       </c>
       <c r="D45" t="n">
-        <v>6.185347902461279</v>
+        <v>4.677656171601808</v>
       </c>
       <c r="E45" t="n">
-        <v>-9.269366245407106</v>
+        <v>-9.269366245407104</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>4.677656171601807</v>
+        <v>13.5818674602828</v>
       </c>
       <c r="I45" t="n">
-        <v>-0.3651549567261063</v>
+        <v>-0.365154956726105</v>
       </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
@@ -2031,10 +2031,10 @@
         <v>0.584895418</v>
       </c>
       <c r="D46" t="n">
-        <v>9.647959552307764</v>
+        <v>9.632950178470395</v>
       </c>
       <c r="E46" t="n">
-        <v>-3.252503968400179</v>
+        <v>-3.252503968400178</v>
       </c>
       <c r="F46" t="n">
         <v>1.736723185428198e-06</v>
@@ -2043,10 +2043,10 @@
         <v>-2.050809446300654</v>
       </c>
       <c r="H46" t="n">
-        <v>9.632950178470395</v>
+        <v>12.77946002393264</v>
       </c>
       <c r="I46" t="n">
-        <v>-0.1059941229379308</v>
+        <v>-0.1059941229379301</v>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
@@ -2064,15 +2064,15 @@
         <v>0.464187656</v>
       </c>
       <c r="D47" t="n">
-        <v>2.284343103950429</v>
+        <v>-0.04312166362878056</v>
       </c>
       <c r="E47" t="n">
-        <v>-11.84634982642061</v>
+        <v>-11.8463498264206</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>-0.04312166362878234</v>
+        <v>10.35138281364132</v>
       </c>
       <c r="I47" t="n">
         <v>-1.451845349150501</v>
@@ -2093,10 +2093,10 @@
         <v>0.504220588</v>
       </c>
       <c r="D48" t="n">
-        <v>4.492915494120616</v>
+        <v>5.450096855694061</v>
       </c>
       <c r="E48" t="n">
-        <v>-7.393000167752932</v>
+        <v>-7.39300016775293</v>
       </c>
       <c r="F48" t="n">
         <v>1.736723185428198e-06</v>
@@ -2105,10 +2105,10 @@
         <v>-3.346265329826826</v>
       </c>
       <c r="H48" t="n">
-        <v>5.450096855694062</v>
+        <v>12.5325814188397</v>
       </c>
       <c r="I48" t="n">
-        <v>-0.3105156046072903</v>
+        <v>-0.3105156046072892</v>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
@@ -2126,10 +2126,10 @@
         <v>0.558489824</v>
       </c>
       <c r="D49" t="n">
-        <v>17.32128453599981</v>
+        <v>16.5712511836367</v>
       </c>
       <c r="E49" t="n">
-        <v>0.9687446217745046</v>
+        <v>0.9687446217745062</v>
       </c>
       <c r="F49" t="n">
         <v>3.473446370856396e-06</v>
@@ -2138,10 +2138,10 @@
         <v>-0.1763403283845134</v>
       </c>
       <c r="H49" t="n">
-        <v>16.5712511836367</v>
+        <v>15.62879530148034</v>
       </c>
       <c r="I49" t="n">
-        <v>0.02628873961814571</v>
+        <v>0.02628873961814593</v>
       </c>
       <c r="J49" t="n">
         <v>1.287385378813148e-05</v>
@@ -2163,18 +2163,18 @@
         <v>0.560142604</v>
       </c>
       <c r="D50" t="n">
-        <v>9.727850191986921</v>
+        <v>9.744475174887114</v>
       </c>
       <c r="E50" t="n">
-        <v>-3.364140110546205</v>
+        <v>-3.364140110546203</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>9.744475174887114</v>
+        <v>12.940556164606</v>
       </c>
       <c r="I50" t="n">
-        <v>-0.1680591208273148</v>
+        <v>-0.168059120827315</v>
       </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
@@ -2192,10 +2192,10 @@
         <v>0.524887769</v>
       </c>
       <c r="D51" t="n">
-        <v>3.028024592936034</v>
+        <v>3.19015705912469</v>
       </c>
       <c r="E51" t="n">
-        <v>-9.988936645456672</v>
+        <v>-9.988936645456667</v>
       </c>
       <c r="F51" t="n">
         <v>1.389378548342558e-05</v>
@@ -2204,10 +2204,10 @@
         <v>-0.5455741380502322</v>
       </c>
       <c r="H51" t="n">
-        <v>3.190157059124689</v>
+        <v>12.65066150925681</v>
       </c>
       <c r="I51" t="n">
-        <v>-0.5284321953245449</v>
+        <v>-0.5284321953245431</v>
       </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
@@ -2225,10 +2225,10 @@
         <v>0.481698311</v>
       </c>
       <c r="D52" t="n">
-        <v>4.21944209839252</v>
+        <v>3.887200865728969</v>
       </c>
       <c r="E52" t="n">
-        <v>-8.828320885929461</v>
+        <v>-8.828320885929458</v>
       </c>
       <c r="F52" t="n">
         <v>8.683615927140989e-07</v>
@@ -2237,10 +2237,10 @@
         <v>-3.591377827663357</v>
       </c>
       <c r="H52" t="n">
-        <v>3.887200865728968</v>
+        <v>12.27047449964756</v>
       </c>
       <c r="I52" t="n">
-        <v>-0.4450472520108668</v>
+        <v>-0.4450472520108657</v>
       </c>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
@@ -2258,15 +2258,15 @@
         <v>0.467282229</v>
       </c>
       <c r="D53" t="n">
-        <v>8.40601182102669</v>
+        <v>8.068973851125318</v>
       </c>
       <c r="E53" t="n">
-        <v>-6.021492597517405</v>
+        <v>-6.021492597517403</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>8.068973851125319</v>
+        <v>12.96500470795793</v>
       </c>
       <c r="I53" t="n">
         <v>-1.125461740684786</v>
@@ -2287,10 +2287,10 @@
         <v>0.553490925</v>
       </c>
       <c r="D54" t="n">
-        <v>13.19808990807823</v>
+        <v>13.81236353833143</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.5299936200610651</v>
+        <v>-0.5299936200610653</v>
       </c>
       <c r="F54" t="n">
         <v>8.683615927140989e-07</v>
@@ -2299,10 +2299,10 @@
         <v>-1.176340328384514</v>
       </c>
       <c r="H54" t="n">
-        <v>13.81236353833143</v>
+        <v>14.04025181893629</v>
       </c>
       <c r="I54" t="n">
-        <v>-0.3021053394561988</v>
+        <v>-0.3021053394562006</v>
       </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
@@ -2320,7 +2320,7 @@
         <v>0.403321877</v>
       </c>
       <c r="D55" t="n">
-        <v>9.344328630286537</v>
+        <v>7.721173906627175</v>
       </c>
       <c r="E55" t="n">
         <v>-6.148882735854456</v>
@@ -2332,10 +2332,10 @@
         <v>-2.91330592255072</v>
       </c>
       <c r="H55" t="n">
-        <v>7.721173906627175</v>
+        <v>13.37063521969007</v>
       </c>
       <c r="I55" t="n">
-        <v>-0.4994214227915619</v>
+        <v>-0.4994214227915621</v>
       </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
@@ -2353,10 +2353,10 @@
         <v>0.48924445</v>
       </c>
       <c r="D56" t="n">
-        <v>9.269388529576446</v>
+        <v>8.010112500213243</v>
       </c>
       <c r="E56" t="n">
-        <v>-7.02905777212584</v>
+        <v>-7.029057772125838</v>
       </c>
       <c r="F56" t="n">
         <v>8.683615927140989e-07</v>
@@ -2365,10 +2365,10 @@
         <v>-2.761302829105669</v>
       </c>
       <c r="H56" t="n">
-        <v>8.010112500213243</v>
+        <v>14.4656148288049</v>
       </c>
       <c r="I56" t="n">
-        <v>-0.5735554435341848</v>
+        <v>-0.5735554435341843</v>
       </c>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
@@ -2386,18 +2386,18 @@
         <v>0.421698894</v>
       </c>
       <c r="D57" t="n">
-        <v>15.18411503784799</v>
+        <v>14.27102271082316</v>
       </c>
       <c r="E57" t="n">
-        <v>-1.85770026930952</v>
+        <v>-1.857700269309519</v>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>14.27102271082316</v>
+        <v>15.63930846252772</v>
       </c>
       <c r="I57" t="n">
-        <v>-0.4894145176049618</v>
+        <v>-0.4894145176049631</v>
       </c>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
@@ -2415,7 +2415,7 @@
         <v>0.317331514</v>
       </c>
       <c r="D58" t="n">
-        <v>12.12507071615625</v>
+        <v>10.61860871541032</v>
       </c>
       <c r="E58" t="n">
         <v>-3.961569885558605</v>
@@ -2423,10 +2423,10 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>10.61860871541032</v>
+        <v>13.80617063219902</v>
       </c>
       <c r="I58" t="n">
-        <v>-0.7740079687698975</v>
+        <v>-0.7740079687698995</v>
       </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
@@ -2444,7 +2444,7 @@
         <v>0.332672477</v>
       </c>
       <c r="D59" t="n">
-        <v>11.63479820484457</v>
+        <v>12.38325472146277</v>
       </c>
       <c r="E59" t="n">
         <v>-3.593546478328274</v>
@@ -2456,10 +2456,10 @@
         <v>1.271118648586708</v>
       </c>
       <c r="H59" t="n">
-        <v>12.38325472146277</v>
+        <v>15.51856988518849</v>
       </c>
       <c r="I59" t="n">
-        <v>-0.4582313146025547</v>
+        <v>-0.4582313146025552</v>
       </c>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
@@ -2477,10 +2477,10 @@
         <v>0.43069784</v>
       </c>
       <c r="D60" t="n">
-        <v>6.024208066198947</v>
+        <v>6.915033594442186</v>
       </c>
       <c r="E60" t="n">
-        <v>-6.965133233092811</v>
+        <v>-6.965133233092807</v>
       </c>
       <c r="F60" t="n">
         <v>2.605084778142297e-06</v>
@@ -2489,10 +2489,10 @@
         <v>-0.5913778276633571</v>
       </c>
       <c r="H60" t="n">
-        <v>6.915033594442185</v>
+        <v>13.57406160196382</v>
       </c>
       <c r="I60" t="n">
-        <v>-0.3061052255711727</v>
+        <v>-0.3061052255711711</v>
       </c>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
@@ -2510,18 +2510,18 @@
         <v>0.468257689</v>
       </c>
       <c r="D61" t="n">
-        <v>9.378766589030075</v>
+        <v>10.065667974418</v>
       </c>
       <c r="E61" t="n">
-        <v>-5.631213007999293</v>
+        <v>-5.631213007999292</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>10.065667974418</v>
+        <v>15.37282343184918</v>
       </c>
       <c r="I61" t="n">
-        <v>-0.32405755056812</v>
+        <v>-0.3240575505681202</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
@@ -2539,18 +2539,18 @@
         <v>0.235812214</v>
       </c>
       <c r="D62" t="n">
-        <v>3.827552061293562</v>
+        <v>3.883861942378701</v>
       </c>
       <c r="E62" t="n">
-        <v>-8.008506176926375</v>
+        <v>-8.008506176926371</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>3.8838619423787</v>
+        <v>10.36375654500825</v>
       </c>
       <c r="I62" t="n">
-        <v>-1.528611574296824</v>
+        <v>-1.528611574296823</v>
       </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
@@ -2568,10 +2568,10 @@
         <v>0.423708475</v>
       </c>
       <c r="D63" t="n">
-        <v>8.11924940966791</v>
+        <v>7.459984682547423</v>
       </c>
       <c r="E63" t="n">
-        <v>-6.074528113362956</v>
+        <v>-6.074528113362954</v>
       </c>
       <c r="F63" t="n">
         <v>4.341807963570494e-06</v>
@@ -2580,7 +2580,7 @@
         <v>0.7305502672240051</v>
       </c>
       <c r="H63" t="n">
-        <v>7.459984682547421</v>
+        <v>13.21218344617723</v>
       </c>
       <c r="I63" t="n">
         <v>-0.3223293497331468</v>
@@ -2601,18 +2601,18 @@
         <v>0.335473079</v>
       </c>
       <c r="D64" t="n">
-        <v>8.20169625531538</v>
+        <v>8.529283775704425</v>
       </c>
       <c r="E64" t="n">
-        <v>-4.058390986055884</v>
+        <v>-4.058390986055885</v>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>8.529283775704426</v>
+        <v>12.16555603512687</v>
       </c>
       <c r="I64" t="n">
-        <v>-0.4221187266334421</v>
+        <v>-0.4221187266334434</v>
       </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
@@ -2630,7 +2630,7 @@
         <v>0.440463938</v>
       </c>
       <c r="D65" t="n">
-        <v>10.14296240833937</v>
+        <v>10.26670366666087</v>
       </c>
       <c r="E65" t="n">
         <v>-3.182457534955237</v>
@@ -2642,10 +2642,10 @@
         <v>0.6716565781704369</v>
       </c>
       <c r="H65" t="n">
-        <v>10.26670366666087</v>
+        <v>12.81889490196887</v>
       </c>
       <c r="I65" t="n">
-        <v>-0.6302662996472307</v>
+        <v>-0.6302662996472309</v>
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
@@ -2663,10 +2663,10 @@
         <v>0.294121152</v>
       </c>
       <c r="D66" t="n">
-        <v>11.30810541005523</v>
+        <v>12.14539756530341</v>
       </c>
       <c r="E66" t="n">
-        <v>-3.500541476163078</v>
+        <v>-3.500541476163075</v>
       </c>
       <c r="F66" t="n">
         <v>8.683615927140989e-07</v>
@@ -2675,10 +2675,10 @@
         <v>-2.591377827663357</v>
       </c>
       <c r="H66" t="n">
-        <v>12.14539756530341</v>
+        <v>14.74587131904596</v>
       </c>
       <c r="I66" t="n">
-        <v>-0.9000677224205247</v>
+        <v>-0.9000677224205231</v>
       </c>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
@@ -2696,10 +2696,10 @@
         <v>0.433967886</v>
       </c>
       <c r="D67" t="n">
-        <v>14.03653533309956</v>
+        <v>14.25548349653589</v>
       </c>
       <c r="E67" t="n">
-        <v>-2.144863523659788</v>
+        <v>-2.144863523659787</v>
       </c>
       <c r="F67" t="n">
         <v>1.736723185428198e-06</v>
@@ -2708,10 +2708,10 @@
         <v>-2.678840668913697</v>
       </c>
       <c r="H67" t="n">
-        <v>14.25548349653589</v>
+        <v>16.03950887060596</v>
       </c>
       <c r="I67" t="n">
-        <v>-0.360838149589719</v>
+        <v>-0.3608381495897197</v>
       </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
@@ -2729,18 +2729,18 @@
         <v>0.404368644</v>
       </c>
       <c r="D68" t="n">
-        <v>10.12102131861062</v>
+        <v>10.65278613007859</v>
       </c>
       <c r="E68" t="n">
-        <v>-4.540562680606902</v>
+        <v>-4.540562680606897</v>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>10.65278613007859</v>
+        <v>15.00641625846313</v>
       </c>
       <c r="I68" t="n">
-        <v>-0.1869325522223577</v>
+        <v>-0.1869325522223557</v>
       </c>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
@@ -2758,7 +2758,7 @@
         <v>0.243562496</v>
       </c>
       <c r="D69" t="n">
-        <v>2.625928032200829</v>
+        <v>0.7282636210301494</v>
       </c>
       <c r="E69" t="n">
         <v>-12.37847365879339</v>
@@ -2766,7 +2766,7 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>0.7282636210301503</v>
+        <v>10.92716328375705</v>
       </c>
       <c r="I69" t="n">
         <v>-2.17957399606648</v>
@@ -2787,7 +2787,7 @@
         <v>0.454888225</v>
       </c>
       <c r="D70" t="n">
-        <v>3.231129257893824</v>
+        <v>2.282635128447745</v>
       </c>
       <c r="E70" t="n">
         <v>-10.26859236748521</v>
@@ -2799,10 +2799,10 @@
         <v>0.9935846730577991</v>
       </c>
       <c r="H70" t="n">
-        <v>2.282635128447745</v>
+        <v>11.5925298019141</v>
       </c>
       <c r="I70" t="n">
-        <v>-0.9586976940188544</v>
+        <v>-0.9586976940188537</v>
       </c>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
@@ -2820,7 +2820,7 @@
         <v>0.7681984120000001</v>
       </c>
       <c r="D71" t="n">
-        <v>4.543427670463085</v>
+        <v>5.330430744524403</v>
       </c>
       <c r="E71" t="n">
         <v>-6.833441600343041</v>
@@ -2828,10 +2828,10 @@
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>5.330430744524403</v>
+        <v>12.15589795031265</v>
       </c>
       <c r="I71" t="n">
-        <v>-0.007974394554787823</v>
+        <v>-0.007974394554788544</v>
       </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
@@ -2849,10 +2849,10 @@
         <v>0.572206553</v>
       </c>
       <c r="D72" t="n">
-        <v>7.558763733150995</v>
+        <v>7.244830263202964</v>
       </c>
       <c r="E72" t="n">
-        <v>-6.096046700624059</v>
+        <v>-6.096046700624055</v>
       </c>
       <c r="F72" t="n">
         <v>8.683615927140989e-07</v>
@@ -2861,10 +2861,10 @@
         <v>-1.176340328384514</v>
       </c>
       <c r="H72" t="n">
-        <v>7.244830263202963</v>
+        <v>13.46687605617228</v>
       </c>
       <c r="I72" t="n">
-        <v>0.1259990923452561</v>
+        <v>0.1259990923452587</v>
       </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
@@ -2882,7 +2882,7 @@
         <v>0.310957437</v>
       </c>
       <c r="D73" t="n">
-        <v>5.913503459025839</v>
+        <v>3.937704483914213</v>
       </c>
       <c r="E73" t="n">
         <v>-10.92096978930029</v>
@@ -2894,10 +2894,10 @@
         <v>-3.983695250442117</v>
       </c>
       <c r="H73" t="n">
-        <v>3.937704483914212</v>
+        <v>13.70576338357865</v>
       </c>
       <c r="I73" t="n">
-        <v>-1.152910889635854</v>
+        <v>-1.152910889635853</v>
       </c>
       <c r="J73" t="n">
         <v>1.170350344375589e-06</v>
@@ -2919,10 +2919,10 @@
         <v>0.496924991</v>
       </c>
       <c r="D74" t="n">
-        <v>17.58883436146456</v>
+        <v>15.56620351631875</v>
       </c>
       <c r="E74" t="n">
-        <v>-0.2747738524513519</v>
+        <v>-0.2747738524513517</v>
       </c>
       <c r="F74" t="n">
         <v>1.997231663242427e-05</v>
@@ -2931,10 +2931,10 @@
         <v>-0.4601332943851044</v>
       </c>
       <c r="H74" t="n">
-        <v>15.56620351631875</v>
+        <v>15.80579192396723</v>
       </c>
       <c r="I74" t="n">
-        <v>-0.03518544480287189</v>
+        <v>-0.03518544480287389</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
@@ -2952,10 +2952,10 @@
         <v>0.341843245</v>
       </c>
       <c r="D75" t="n">
-        <v>8.446426226825633</v>
+        <v>9.555375105847418</v>
       </c>
       <c r="E75" t="n">
-        <v>-5.635557377856918</v>
+        <v>-5.635557377856915</v>
       </c>
       <c r="F75" t="n">
         <v>8.683615927140989e-07</v>
@@ -2964,7 +2964,7 @@
         <v>-3.761302829105669</v>
       </c>
       <c r="H75" t="n">
-        <v>9.555375105847418</v>
+        <v>14.14360699219884</v>
       </c>
       <c r="I75" t="n">
         <v>-1.047325491505492</v>
@@ -2985,18 +2985,18 @@
         <v>0.492776546</v>
       </c>
       <c r="D76" t="n">
-        <v>6.378541275116641</v>
+        <v>4.235131808529415</v>
       </c>
       <c r="E76" t="n">
-        <v>-9.369771775333941</v>
+        <v>-9.369771775333938</v>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>4.235131808529414</v>
+        <v>13.02935014981891</v>
       </c>
       <c r="I76" t="n">
-        <v>-0.5755534340444501</v>
+        <v>-0.5755534340444481</v>
       </c>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
@@ -3014,7 +3014,7 @@
         <v>0.501304824</v>
       </c>
       <c r="D77" t="n">
-        <v>20.34614467114585</v>
+        <v>21.81993832794947</v>
       </c>
       <c r="E77" t="n">
         <v>4.850394062388732</v>
@@ -3026,10 +3026,10 @@
         <v>-0.3398390606673928</v>
       </c>
       <c r="H77" t="n">
-        <v>21.81993832794947</v>
+        <v>17.38532177877094</v>
       </c>
       <c r="I77" t="n">
-        <v>0.4157775132102068</v>
+        <v>0.4157775132102051</v>
       </c>
       <c r="J77" t="n">
         <v>0.0001205460854706856</v>
@@ -3051,10 +3051,10 @@
         <v>0.522744307</v>
       </c>
       <c r="D78" t="n">
-        <v>6.4647245534159</v>
+        <v>6.259807198565517</v>
       </c>
       <c r="E78" t="n">
-        <v>-6.951768133970833</v>
+        <v>-6.951768133970831</v>
       </c>
       <c r="F78" t="n">
         <v>4.602316441384724e-05</v>
@@ -3063,7 +3063,7 @@
         <v>1.136542626899842</v>
       </c>
       <c r="H78" t="n">
-        <v>6.259807198565516</v>
+        <v>13.436752347535</v>
       </c>
       <c r="I78" t="n">
         <v>0.2251770149986563</v>
@@ -3084,7 +3084,7 @@
         <v>0.630137883</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.4948044792049424</v>
+        <v>-4.562035244427765</v>
       </c>
       <c r="E79" t="n">
         <v>-15.18220275083886</v>
@@ -3096,10 +3096,10 @@
         <v>0.8742857446854547</v>
       </c>
       <c r="H79" t="n">
-        <v>-4.562035244427763</v>
+        <v>10.50316770751554</v>
       </c>
       <c r="I79" t="n">
-        <v>-0.11699979889556</v>
+        <v>-0.1169997988955604</v>
       </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
@@ -3117,10 +3117,10 @@
         <v>0.404563024</v>
       </c>
       <c r="D80" t="n">
-        <v>11.93038094202008</v>
+        <v>10.53257481703519</v>
       </c>
       <c r="E80" t="n">
-        <v>-4.864926082841749</v>
+        <v>-4.864926082841744</v>
       </c>
       <c r="F80" t="n">
         <v>8.683615927140989e-07</v>
@@ -3129,10 +3129,10 @@
         <v>-3.591377827663357</v>
       </c>
       <c r="H80" t="n">
-        <v>10.53257481703519</v>
+        <v>14.67246039086362</v>
       </c>
       <c r="I80" t="n">
-        <v>-0.7250405090133165</v>
+        <v>-0.7250405090133138</v>
       </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
@@ -3150,10 +3150,10 @@
         <v>0.317470035</v>
       </c>
       <c r="D81" t="n">
-        <v>10.68128550689754</v>
+        <v>10.08473596218145</v>
       </c>
       <c r="E81" t="n">
-        <v>-3.882452654211813</v>
+        <v>-3.882452654211812</v>
       </c>
       <c r="F81" t="n">
         <v>1.736723185428198e-06</v>
@@ -3162,7 +3162,7 @@
         <v>-3.498268423271876</v>
       </c>
       <c r="H81" t="n">
-        <v>10.08473596218145</v>
+        <v>12.92074549033922</v>
       </c>
       <c r="I81" t="n">
         <v>-1.046443126054043</v>
@@ -3183,18 +3183,18 @@
         <v>0.470191968</v>
       </c>
       <c r="D82" t="n">
-        <v>3.276068158658234</v>
+        <v>3.315958991411651</v>
       </c>
       <c r="E82" t="n">
-        <v>-8.899602710754376</v>
+        <v>-8.899602710754374</v>
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
-        <v>3.315958991411651</v>
+        <v>11.5956129556812</v>
       </c>
       <c r="I82" t="n">
-        <v>-0.619948746484821</v>
+        <v>-0.6199487464848215</v>
       </c>
       <c r="J82" t="n">
         <v>1.170350344375589e-06</v>
@@ -3216,7 +3216,7 @@
         <v>0.573824449</v>
       </c>
       <c r="D83" t="n">
-        <v>2.224358719593472</v>
+        <v>0.1259356123694182</v>
       </c>
       <c r="E83" t="n">
         <v>-10.65962315711549</v>
@@ -3228,10 +3228,10 @@
         <v>1.730550267224005</v>
       </c>
       <c r="H83" t="n">
-        <v>0.1259356123694175</v>
+        <v>10.84303168236413</v>
       </c>
       <c r="I83" t="n">
-        <v>0.05747291287922252</v>
+        <v>0.05747291287922274</v>
       </c>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
@@ -3249,10 +3249,10 @@
         <v>0.408548449</v>
       </c>
       <c r="D84" t="n">
-        <v>17.83205980248395</v>
+        <v>19.13239754639152</v>
       </c>
       <c r="E84" t="n">
-        <v>1.623053620690787</v>
+        <v>1.623053620690789</v>
       </c>
       <c r="F84" t="n">
         <v>1.736723185428198e-05</v>
@@ -3261,10 +3261,10 @@
         <v>-0.554851951638243</v>
       </c>
       <c r="H84" t="n">
-        <v>19.13239754639152</v>
+        <v>17.52600308348096</v>
       </c>
       <c r="I84" t="n">
-        <v>0.01665915778023264</v>
+        <v>0.01665915778023397</v>
       </c>
       <c r="J84" t="n">
         <v>1.638490482125824e-05</v>
@@ -3286,10 +3286,10 @@
         <v>0.598444177</v>
       </c>
       <c r="D85" t="n">
-        <v>20.15917235209383</v>
+        <v>20.64329527154715</v>
       </c>
       <c r="E85" t="n">
-        <v>4.846593031871142</v>
+        <v>4.846593031871143</v>
       </c>
       <c r="F85" t="n">
         <v>5.383841874827413e-05</v>
@@ -3298,7 +3298,7 @@
         <v>0.4559278871149994</v>
       </c>
       <c r="H85" t="n">
-        <v>20.64329527154715</v>
+        <v>15.99686090380953</v>
       </c>
       <c r="I85" t="n">
         <v>0.2001586641335227</v>
@@ -3323,10 +3323,10 @@
         <v>0.665391251</v>
       </c>
       <c r="D86" t="n">
-        <v>19.31528922293637</v>
+        <v>19.44321956252464</v>
       </c>
       <c r="E86" t="n">
-        <v>2.679982560502484</v>
+        <v>2.679982560502483</v>
       </c>
       <c r="F86" t="n">
         <v>8.683615927140989e-06</v>
@@ -3335,10 +3335,10 @@
         <v>0.9231953451664011</v>
       </c>
       <c r="H86" t="n">
-        <v>19.44321956252464</v>
+        <v>17.51814402493251</v>
       </c>
       <c r="I86" t="n">
-        <v>0.7549070229103652</v>
+        <v>0.7549070229103636</v>
       </c>
       <c r="J86" t="n">
         <v>6.085821790753062e-05</v>
@@ -3360,7 +3360,7 @@
         <v>0.497581594</v>
       </c>
       <c r="D87" t="n">
-        <v>19.39428639902644</v>
+        <v>19.21146202954246</v>
       </c>
       <c r="E87" t="n">
         <v>3.646604166417159</v>
@@ -3372,10 +3372,10 @@
         <v>0.2451234400537635</v>
       </c>
       <c r="H87" t="n">
-        <v>19.21146202954247</v>
+        <v>16.03268281645457</v>
       </c>
       <c r="I87" t="n">
-        <v>0.4678249533292658</v>
+        <v>0.4678249533292647</v>
       </c>
       <c r="J87" t="n">
         <v>0.0003721714095114373</v>
@@ -3397,10 +3397,10 @@
         <v>0.611622504</v>
       </c>
       <c r="D88" t="n">
-        <v>21.66370967331818</v>
+        <v>20.78428220439769</v>
       </c>
       <c r="E88" t="n">
-        <v>4.561057304958099</v>
+        <v>4.5610573049581</v>
       </c>
       <c r="F88" t="n">
         <v>0.0003377926595657845</v>
@@ -3409,10 +3409,10 @@
         <v>1.764321003879249</v>
       </c>
       <c r="H88" t="n">
-        <v>20.78428220439769</v>
+        <v>16.72153745380217</v>
       </c>
       <c r="I88" t="n">
-        <v>0.4983125543625784</v>
+        <v>0.4983125543625782</v>
       </c>
       <c r="J88" t="n">
         <v>0.007322882104758059</v>
@@ -3434,10 +3434,10 @@
         <v>0.466704263</v>
       </c>
       <c r="D89" t="n">
-        <v>22.84869180063464</v>
+        <v>22.55241826879008</v>
       </c>
       <c r="E89" t="n">
-        <v>4.028996707839014</v>
+        <v>4.028996707839013</v>
       </c>
       <c r="F89" t="n">
         <v>0.000158041809873966</v>
@@ -3446,10 +3446,10 @@
         <v>0.9277321257631733</v>
       </c>
       <c r="H89" t="n">
-        <v>22.55241826879008</v>
+        <v>18.82696948754088</v>
       </c>
       <c r="I89" t="n">
-        <v>0.3035479265898153</v>
+        <v>0.3035479265898129</v>
       </c>
       <c r="J89" t="n">
         <v>0.002773730316170145</v>
@@ -3471,10 +3471,10 @@
         <v>0.6796563839999999</v>
       </c>
       <c r="D90" t="n">
-        <v>23.80723324239702</v>
+        <v>23.54790193612411</v>
       </c>
       <c r="E90" t="n">
-        <v>4.587776230702329</v>
+        <v>4.587776230702331</v>
       </c>
       <c r="F90" t="n">
         <v>5.818022671184463e-05</v>
@@ -3483,10 +3483,10 @@
         <v>0.4303172434359618</v>
       </c>
       <c r="H90" t="n">
-        <v>23.54790193612411</v>
+        <v>19.39370739571533</v>
       </c>
       <c r="I90" t="n">
-        <v>0.4335816902935472</v>
+        <v>0.4335816902935463</v>
       </c>
       <c r="J90" t="n">
         <v>0.0007993492852085271</v>
@@ -3508,10 +3508,10 @@
         <v>0.557079152</v>
       </c>
       <c r="D91" t="n">
-        <v>20.90511187561675</v>
+        <v>20.46695203319463</v>
       </c>
       <c r="E91" t="n">
-        <v>4.677282950777611</v>
+        <v>4.677282950777613</v>
       </c>
       <c r="F91" t="n">
         <v>4.341807963570494e-06</v>
@@ -3520,10 +3520,10 @@
         <v>0.1455877665028488</v>
       </c>
       <c r="H91" t="n">
-        <v>20.46695203319463</v>
+        <v>16.15454494125146</v>
       </c>
       <c r="I91" t="n">
-        <v>0.3648758588344405</v>
+        <v>0.3648758588344401</v>
       </c>
       <c r="J91" t="n">
         <v>0.0002750323309282634</v>
@@ -3545,7 +3545,7 @@
         <v>0.602225174</v>
       </c>
       <c r="D92" t="n">
-        <v>20.16117395154208</v>
+        <v>19.31299628409622</v>
       </c>
       <c r="E92" t="n">
         <v>3.551075877309152</v>
@@ -3557,10 +3557,10 @@
         <v>1.059037734546415</v>
       </c>
       <c r="H92" t="n">
-        <v>19.31299628409621</v>
+        <v>16.23151027051814</v>
       </c>
       <c r="I92" t="n">
-        <v>0.4695898637310769</v>
+        <v>0.4695898637310767</v>
       </c>
       <c r="J92" t="n">
         <v>0.004586602999607932</v>
@@ -3582,10 +3582,10 @@
         <v>0.580088966</v>
       </c>
       <c r="D93" t="n">
-        <v>19.82455508922603</v>
+        <v>19.3758177425279</v>
       </c>
       <c r="E93" t="n">
-        <v>2.321334824279697</v>
+        <v>2.321334824279698</v>
       </c>
       <c r="F93" t="n">
         <v>1.389378548342558e-05</v>
@@ -3594,7 +3594,7 @@
         <v>0.5017315767281243</v>
       </c>
       <c r="H93" t="n">
-        <v>19.3758177425279</v>
+        <v>17.38233902370263</v>
       </c>
       <c r="I93" t="n">
         <v>0.3278561054544376</v>
@@ -3619,10 +3619,10 @@
         <v>0.425541894</v>
       </c>
       <c r="D94" t="n">
-        <v>20.16498291209622</v>
+        <v>19.84008398578937</v>
       </c>
       <c r="E94" t="n">
-        <v>3.483511751659216</v>
+        <v>3.483511751659217</v>
       </c>
       <c r="F94" t="n">
         <v>2.518248618870887e-05</v>
@@ -3631,10 +3631,10 @@
         <v>0.05714980183526538</v>
       </c>
       <c r="H94" t="n">
-        <v>19.84008398578937</v>
+        <v>16.36430570508444</v>
       </c>
       <c r="I94" t="n">
-        <v>0.007733470954283117</v>
+        <v>0.007733470954281341</v>
       </c>
       <c r="J94" t="n">
         <v>0.0003522754536570522</v>
@@ -3656,10 +3656,10 @@
         <v>0.661500447</v>
       </c>
       <c r="D95" t="n">
-        <v>18.4979983006413</v>
+        <v>19.13388324359203</v>
       </c>
       <c r="E95" t="n">
-        <v>4.169268552535678</v>
+        <v>4.169268552535679</v>
       </c>
       <c r="F95" t="n">
         <v>0.0001198338997945457</v>
@@ -3668,10 +3668,10 @@
         <v>1.472752509756359</v>
       </c>
       <c r="H95" t="n">
-        <v>19.13388324359203</v>
+        <v>15.4076824667096</v>
       </c>
       <c r="I95" t="n">
-        <v>0.4430677756532511</v>
+        <v>0.4430677756532504</v>
       </c>
       <c r="J95" t="n">
         <v>0.001337710443621298</v>
@@ -3693,10 +3693,10 @@
         <v>0.518502705</v>
       </c>
       <c r="D96" t="n">
-        <v>18.44121466635465</v>
+        <v>16.72898384748754</v>
       </c>
       <c r="E96" t="n">
-        <v>0.09213226907106498</v>
+        <v>0.09213226907106631</v>
       </c>
       <c r="F96" t="n">
         <v>6.946892741712791e-06</v>
@@ -3705,10 +3705,10 @@
         <v>-0.05080944630065446</v>
       </c>
       <c r="H96" t="n">
-        <v>16.72898384748754</v>
+        <v>16.99333791382486</v>
       </c>
       <c r="I96" t="n">
-        <v>0.3564863354083871</v>
+        <v>0.3564863354083869</v>
       </c>
       <c r="J96" t="n">
         <v>3.511051033126766e-05</v>
@@ -3730,10 +3730,10 @@
         <v>0.576817585</v>
       </c>
       <c r="D97" t="n">
-        <v>20.51426446001431</v>
+        <v>19.22345797784778</v>
       </c>
       <c r="E97" t="n">
-        <v>2.565876245399096</v>
+        <v>2.565876245399097</v>
       </c>
       <c r="F97" t="n">
         <v>6.946892741712791e-06</v>
@@ -3742,10 +3742,10 @@
         <v>-0.2918175458044493</v>
       </c>
       <c r="H97" t="n">
-        <v>19.22345797784778</v>
+        <v>17.1229906934518</v>
       </c>
       <c r="I97" t="n">
-        <v>0.4654089610031198</v>
+        <v>0.4654089610031187</v>
       </c>
       <c r="J97" t="n">
         <v>6.202856825190622e-05</v>
@@ -3767,10 +3767,10 @@
         <v>0.49441288</v>
       </c>
       <c r="D98" t="n">
-        <v>21.82410040762652</v>
+        <v>21.2118843362794</v>
       </c>
       <c r="E98" t="n">
-        <v>3.171008216561438</v>
+        <v>3.171008216561439</v>
       </c>
       <c r="F98" t="n">
         <v>9.551977519855087e-06</v>
@@ -3779,10 +3779,10 @@
         <v>-0.03883680463457864</v>
       </c>
       <c r="H98" t="n">
-        <v>21.2118843362794</v>
+        <v>18.23536628934741</v>
       </c>
       <c r="I98" t="n">
-        <v>0.1944901696294399</v>
+        <v>0.194490169629439</v>
       </c>
       <c r="J98" t="n">
         <v>0.0001217164358150612</v>
@@ -3804,10 +3804,10 @@
         <v>0.6741516</v>
       </c>
       <c r="D99" t="n">
-        <v>20.99355380703233</v>
+        <v>20.67691923524711</v>
       </c>
       <c r="E99" t="n">
-        <v>3.171549220472684</v>
+        <v>3.171549220472687</v>
       </c>
       <c r="F99" t="n">
         <v>0.0001042033911256919</v>
@@ -3816,10 +3816,10 @@
         <v>1.48262275378042</v>
       </c>
       <c r="H99" t="n">
-        <v>20.67691923524711</v>
+        <v>17.95338632787417</v>
       </c>
       <c r="I99" t="n">
-        <v>0.4480163130997454</v>
+        <v>0.4480163130997457</v>
       </c>
       <c r="J99" t="n">
         <v>0.0008918069624141987</v>
@@ -3841,10 +3841,10 @@
         <v>0.504493586</v>
       </c>
       <c r="D100" t="n">
-        <v>22.18856547443391</v>
+        <v>21.39912884983688</v>
       </c>
       <c r="E100" t="n">
-        <v>2.595683755447868</v>
+        <v>2.595683755447869</v>
       </c>
       <c r="F100" t="n">
         <v>0.0003143468965625038</v>
@@ -3853,10 +3853,10 @@
         <v>0.582038572297545</v>
       </c>
       <c r="H100" t="n">
-        <v>21.39912884983688</v>
+        <v>19.04654748003089</v>
       </c>
       <c r="I100" t="n">
-        <v>0.243102385641879</v>
+        <v>0.2431023856418781</v>
       </c>
       <c r="J100" t="n">
         <v>0.003221974498065996</v>
@@ -3878,10 +3878,10 @@
         <v>0.623300738</v>
       </c>
       <c r="D101" t="n">
-        <v>22.15278315965208</v>
+        <v>21.88605803047528</v>
       </c>
       <c r="E101" t="n">
-        <v>2.935972141374079</v>
+        <v>2.935972141374082</v>
       </c>
       <c r="F101" t="n">
         <v>1.649887026156788e-05</v>
@@ -3890,10 +3890,10 @@
         <v>0.4866246843379161</v>
       </c>
       <c r="H101" t="n">
-        <v>21.88605803047528</v>
+        <v>19.09102926709085</v>
       </c>
       <c r="I101" t="n">
-        <v>0.1409433779896485</v>
+        <v>0.1409433779896487</v>
       </c>
       <c r="J101" t="n">
         <v>9.713907858317387e-05</v>
@@ -3915,10 +3915,10 @@
         <v>0.652863485</v>
       </c>
       <c r="D102" t="n">
-        <v>21.26957694242414</v>
+        <v>20.6541965467521</v>
       </c>
       <c r="E102" t="n">
-        <v>4.101958489664042</v>
+        <v>4.101958489664043</v>
       </c>
       <c r="F102" t="n">
         <v>2.952429415227936e-05</v>
@@ -3927,10 +3927,10 @@
         <v>1.79564529544589</v>
       </c>
       <c r="H102" t="n">
-        <v>20.6541965467521</v>
+        <v>16.96572613193494</v>
       </c>
       <c r="I102" t="n">
-        <v>0.4134880748468797</v>
+        <v>0.4134880748468792</v>
       </c>
       <c r="J102" t="n">
         <v>0.0002141741130207327</v>
@@ -3952,10 +3952,10 @@
         <v>0.581703122</v>
       </c>
       <c r="D103" t="n">
-        <v>18.31699042015724</v>
+        <v>17.00594582607346</v>
       </c>
       <c r="E103" t="n">
-        <v>1.938154385302203</v>
+        <v>1.938154385302206</v>
       </c>
       <c r="F103" t="n">
         <v>5.210169556284594e-06</v>
@@ -3964,10 +3964,10 @@
         <v>-0.4658469455794983</v>
       </c>
       <c r="H103" t="n">
-        <v>17.00594582607346</v>
+        <v>15.23897831426211</v>
       </c>
       <c r="I103" t="n">
-        <v>0.1711868734908517</v>
+        <v>0.1711868734908519</v>
       </c>
       <c r="J103" t="n">
         <v>8.543557513941798e-05</v>
@@ -3989,10 +3989,10 @@
         <v>0.752652305</v>
       </c>
       <c r="D104" t="n">
-        <v>22.32206772812104</v>
+        <v>23.07494644811731</v>
       </c>
       <c r="E104" t="n">
-        <v>5.146573681899985</v>
+        <v>5.146573681899988</v>
       </c>
       <c r="F104" t="n">
         <v>5.904858830455872e-05</v>
@@ -4001,10 +4001,10 @@
         <v>1.036653394949685</v>
       </c>
       <c r="H104" t="n">
-        <v>23.07494644811731</v>
+        <v>18.64527077863276</v>
       </c>
       <c r="I104" t="n">
-        <v>0.7168980124154445</v>
+        <v>0.716898012415444</v>
       </c>
       <c r="J104" t="n">
         <v>0.00187841230272282</v>
@@ -4026,10 +4026,10 @@
         <v>0.495113639</v>
       </c>
       <c r="D105" t="n">
-        <v>22.41027119916136</v>
+        <v>22.30755258051497</v>
       </c>
       <c r="E105" t="n">
-        <v>4.485906415790653</v>
+        <v>4.485906415790654</v>
       </c>
       <c r="F105" t="n">
         <v>7.81525433442689e-06</v>
@@ -4038,10 +4038,10 @@
         <v>-1.279433821348617</v>
       </c>
       <c r="H105" t="n">
-        <v>22.30755258051497</v>
+        <v>18.03582665341589</v>
       </c>
       <c r="I105" t="n">
-        <v>0.2141804886915779</v>
+        <v>0.2141804886915766</v>
       </c>
       <c r="J105" t="n">
         <v>0.0001661897489013336</v>
@@ -4063,10 +4063,10 @@
         <v>0.494281801</v>
       </c>
       <c r="D106" t="n">
-        <v>23.37864591656501</v>
+        <v>23.33035276225481</v>
       </c>
       <c r="E106" t="n">
-        <v>5.173219317508184</v>
+        <v>5.173219317508185</v>
       </c>
       <c r="F106" t="n">
         <v>2.691920937413706e-05</v>
@@ -4075,10 +4075,10 @@
         <v>-0.02949894005524221</v>
       </c>
       <c r="H106" t="n">
-        <v>23.33035276225481</v>
+        <v>18.47081797856139</v>
       </c>
       <c r="I106" t="n">
-        <v>0.3136845338147691</v>
+        <v>0.3136845338147669</v>
       </c>
       <c r="J106" t="n">
         <v>0.0007291282645459919</v>
@@ -4100,10 +4100,10 @@
         <v>0.575902303</v>
       </c>
       <c r="D107" t="n">
-        <v>20.06727221783684</v>
+        <v>19.62428675504104</v>
       </c>
       <c r="E107" t="n">
-        <v>3.191826912370781</v>
+        <v>3.191826912370783</v>
       </c>
       <c r="F107" t="n">
         <v>1.736723185428198e-06</v>
@@ -4112,10 +4112,10 @@
         <v>-1.176340328384514</v>
       </c>
       <c r="H107" t="n">
-        <v>19.62428675504104</v>
+        <v>16.5889343981664</v>
       </c>
       <c r="I107" t="n">
-        <v>0.1564745554961422</v>
+        <v>0.1564745554961409</v>
       </c>
       <c r="J107" t="n">
         <v>5.500646618565268e-05</v>
@@ -4137,10 +4137,10 @@
         <v>0.475196965</v>
       </c>
       <c r="D108" t="n">
-        <v>21.02933612181416</v>
+        <v>20.18999005460871</v>
       </c>
       <c r="E108" t="n">
-        <v>2.831260834546473</v>
+        <v>2.831260834546474</v>
       </c>
       <c r="F108" t="n">
         <v>0.0001675937873938211</v>
@@ -4149,10 +4149,10 @@
         <v>1.012394522832557</v>
       </c>
       <c r="H108" t="n">
-        <v>20.18999005460871</v>
+        <v>17.90890454081421</v>
       </c>
       <c r="I108" t="n">
-        <v>0.5501753207519759</v>
+        <v>0.5501753207519751</v>
       </c>
       <c r="J108" t="n">
         <v>0.001741481312430876</v>
@@ -4174,7 +4174,7 @@
         <v>0.502505497</v>
       </c>
       <c r="D109" t="n">
-        <v>23.64540028911302</v>
+        <v>23.30180004506395</v>
       </c>
       <c r="E109" t="n">
         <v>4.30621001710618</v>
@@ -4186,10 +4186,10 @@
         <v>0.3245579075481683</v>
       </c>
       <c r="H109" t="n">
-        <v>23.30180004506395</v>
+        <v>19.50662786232684</v>
       </c>
       <c r="I109" t="n">
-        <v>0.5110378343690674</v>
+        <v>0.5110378343690656</v>
       </c>
       <c r="J109" t="n">
         <v>0.001285044678124397</v>
@@ -4211,10 +4211,10 @@
         <v>0.551943626</v>
       </c>
       <c r="D110" t="n">
-        <v>20.69227310492678</v>
+        <v>20.81188561803199</v>
       </c>
       <c r="E110" t="n">
-        <v>4.632773680182309</v>
+        <v>4.63277368018231</v>
       </c>
       <c r="F110" t="n">
         <v>5.210169556284594e-06</v>
@@ -4223,10 +4223,10 @@
         <v>-0.3283434218295631</v>
       </c>
       <c r="H110" t="n">
-        <v>20.81188561803199</v>
+        <v>16.62937956470086</v>
       </c>
       <c r="I110" t="n">
-        <v>0.4502676268511787</v>
+        <v>0.4502676268511783</v>
       </c>
       <c r="J110" t="n">
         <v>0.0003241870453920381</v>
@@ -4269,10 +4269,10 @@
         <v>0.658613921</v>
       </c>
       <c r="D112" t="n">
-        <v>23.67605200822555</v>
+        <v>24.46875725844992</v>
       </c>
       <c r="E112" t="n">
-        <v>5.588197887207377</v>
+        <v>5.588197887207379</v>
       </c>
       <c r="F112" t="n">
         <v>0.0001154920918309752</v>
@@ -4281,10 +4281,10 @@
         <v>0.4981203231757457</v>
       </c>
       <c r="H112" t="n">
-        <v>24.46875725844992</v>
+        <v>19.59677427516738</v>
       </c>
       <c r="I112" t="n">
-        <v>0.7162149039248387</v>
+        <v>0.7162149039248378</v>
       </c>
       <c r="J112" t="n">
         <v>0.003015992837455892</v>
@@ -4306,7 +4306,7 @@
         <v>0.651996322</v>
       </c>
       <c r="D113" t="n">
-        <v>21.45986257573924</v>
+        <v>21.8406189407292</v>
       </c>
       <c r="E113" t="n">
         <v>3.607802218206481</v>
@@ -4318,10 +4318,10 @@
         <v>0.4086221723366428</v>
       </c>
       <c r="H113" t="n">
-        <v>21.8406189407292</v>
+        <v>18.93052579815172</v>
       </c>
       <c r="I113" t="n">
-        <v>0.6977090756290067</v>
+        <v>0.6977090756290052</v>
       </c>
       <c r="J113" t="n">
         <v>0.0006483740907840762</v>
@@ -4343,10 +4343,10 @@
         <v>0.620917889</v>
       </c>
       <c r="D114" t="n">
-        <v>23.28093522230563</v>
+        <v>23.11455553150648</v>
       </c>
       <c r="E114" t="n">
-        <v>4.881534478219749</v>
+        <v>4.88153447821975</v>
       </c>
       <c r="F114" t="n">
         <v>4.341807963570494e-05</v>
@@ -4355,10 +4355,10 @@
         <v>0.9650155208610282</v>
       </c>
       <c r="H114" t="n">
-        <v>23.11455553150648</v>
+        <v>18.69544667164335</v>
       </c>
       <c r="I114" t="n">
-        <v>0.4624256183566282</v>
+        <v>0.4624256183566264</v>
       </c>
       <c r="J114" t="n">
         <v>0.001354095348442556</v>
@@ -4380,10 +4380,10 @@
         <v>0.712756656</v>
       </c>
       <c r="D115" t="n">
-        <v>24.44259084892692</v>
+        <v>25.36631015521095</v>
       </c>
       <c r="E115" t="n">
-        <v>6.565137294807527</v>
+        <v>6.565137294807529</v>
       </c>
       <c r="F115" t="n">
         <v>0.0001484898323541109</v>
@@ -4392,10 +4392,10 @@
         <v>0.2642322630014681</v>
       </c>
       <c r="H115" t="n">
-        <v>25.36631015521095</v>
+        <v>19.35185659036009</v>
       </c>
       <c r="I115" t="n">
-        <v>0.5506837299566614</v>
+        <v>0.5506837299566618</v>
       </c>
       <c r="J115" t="n">
         <v>0.002451883971466859</v>
@@ -4417,10 +4417,10 @@
         <v>0.640254579</v>
       </c>
       <c r="D116" t="n">
-        <v>20.54967435294749</v>
+        <v>21.15179991290754</v>
       </c>
       <c r="E116" t="n">
-        <v>3.018081612450879</v>
+        <v>3.01808161245088</v>
       </c>
       <c r="F116" t="n">
         <v>0.0001710672337646775</v>
@@ -4429,10 +4429,10 @@
         <v>1.430761149605892</v>
       </c>
       <c r="H116" t="n">
-        <v>21.15179991290754</v>
+        <v>18.95188237548249</v>
       </c>
       <c r="I116" t="n">
-        <v>0.8181640750258288</v>
+        <v>0.8181640750258272</v>
       </c>
       <c r="J116" t="n">
         <v>0.001750844115185881</v>
@@ -4454,7 +4454,7 @@
         <v>0.566632593</v>
       </c>
       <c r="D117" t="n">
-        <v>19.39263351139246</v>
+        <v>19.74574237478612</v>
       </c>
       <c r="E117" t="n">
         <v>3.869653624270993</v>
@@ -4466,10 +4466,10 @@
         <v>-1.465846945579498</v>
       </c>
       <c r="H117" t="n">
-        <v>19.74574237478612</v>
+        <v>16.24177858861682</v>
       </c>
       <c r="I117" t="n">
-        <v>0.3656898381017</v>
+        <v>0.3656898381016986</v>
       </c>
       <c r="J117" t="n">
         <v>0.0002001299088882257</v>
@@ -4491,10 +4491,10 @@
         <v>0.601412868</v>
       </c>
       <c r="D118" t="n">
-        <v>23.91629282883553</v>
+        <v>24.93296375059332</v>
       </c>
       <c r="E118" t="n">
-        <v>6.858895542324946</v>
+        <v>6.858895542324948</v>
       </c>
       <c r="F118" t="n">
         <v>6.339039626812922e-05</v>
@@ -4503,10 +4503,10 @@
         <v>0.3889933655877104</v>
       </c>
       <c r="H118" t="n">
-        <v>24.93296375059332</v>
+        <v>18.65359586628811</v>
       </c>
       <c r="I118" t="n">
-        <v>0.5795276580197424</v>
+        <v>0.5795276580197419</v>
       </c>
       <c r="J118" t="n">
         <v>0.003063977201575291</v>
@@ -4528,7 +4528,7 @@
         <v>0.638649927</v>
       </c>
       <c r="D119" t="n">
-        <v>24.28075789564292</v>
+        <v>25.1202082641508</v>
       </c>
       <c r="E119" t="n">
         <v>6.283571081211377</v>
@@ -4540,10 +4540,10 @@
         <v>0.5272666688352622</v>
       </c>
       <c r="H119" t="n">
-        <v>25.12020826415079</v>
+        <v>19.4647770569716</v>
       </c>
       <c r="I119" t="n">
-        <v>0.6281398740321815</v>
+        <v>0.6281398740321811</v>
       </c>
       <c r="J119" t="n">
         <v>0.002275161069466145</v>
@@ -4565,20 +4565,20 @@
         <v>0.581635233</v>
       </c>
       <c r="D120" t="n">
-        <v>19.32845327213752</v>
+        <v>20.32075356649137</v>
       </c>
       <c r="E120" t="n">
-        <v>4.621963781275957</v>
+        <v>4.62196378127596</v>
       </c>
       <c r="F120" t="n">
         <v>6.078531148998692e-06</v>
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="n">
-        <v>20.32075356649137</v>
+        <v>15.9623159882125</v>
       </c>
       <c r="I120" t="n">
-        <v>0.26352620299709</v>
+        <v>0.2635262029970886</v>
       </c>
       <c r="J120" t="n">
         <v>0.0002539660247295028</v>
@@ -4598,10 +4598,10 @@
         <v>0.548171131</v>
       </c>
       <c r="D121" t="n">
-        <v>24.047474063007</v>
+        <v>24.01210842826751</v>
       </c>
       <c r="E121" t="n">
-        <v>5.858473885819898</v>
+        <v>5.8584738858199</v>
       </c>
       <c r="F121" t="n">
         <v>6.252203467541512e-05</v>
@@ -4610,10 +4610,10 @@
         <v>0.3497284832830745</v>
       </c>
       <c r="H121" t="n">
-        <v>24.01210842826751</v>
+        <v>18.45052898683606</v>
       </c>
       <c r="I121" t="n">
-        <v>0.2968944443884509</v>
+        <v>0.2968944443884505</v>
       </c>
       <c r="J121" t="n">
         <v>0.002010661891637262</v>
@@ -4635,10 +4635,10 @@
         <v>0.610836121</v>
       </c>
       <c r="D122" t="n">
-        <v>22.68338569744918</v>
+        <v>23.53086624973617</v>
       </c>
       <c r="E122" t="n">
-        <v>4.104717983284142</v>
+        <v>4.104717983284144</v>
       </c>
       <c r="F122" t="n">
         <v>5.991694989727283e-05</v>
@@ -4647,10 +4647,10 @@
         <v>-0.2377408730486566</v>
       </c>
       <c r="H122" t="n">
-        <v>23.53086624973617</v>
+        <v>19.97212414208738</v>
       </c>
       <c r="I122" t="n">
-        <v>0.5459758756353494</v>
+        <v>0.5459758756353488</v>
       </c>
       <c r="J122" t="n">
         <v>0.001421975668416341</v>
@@ -4672,10 +4672,10 @@
         <v>0.558968485</v>
       </c>
       <c r="D123" t="n">
-        <v>18.77185498506537</v>
+        <v>18.40739301976334</v>
       </c>
       <c r="E123" t="n">
-        <v>2.967669785126603</v>
+        <v>2.967669785126604</v>
       </c>
       <c r="F123" t="n">
         <v>0.0001154920918309752</v>
@@ -4684,10 +4684,10 @@
         <v>1.020961111989104</v>
       </c>
       <c r="H123" t="n">
-        <v>18.40739301976335</v>
+        <v>15.85862401679311</v>
       </c>
       <c r="I123" t="n">
-        <v>0.4189007821563637</v>
+        <v>0.4189007821563628</v>
       </c>
       <c r="J123" t="n">
         <v>0.001105981075434932</v>
@@ -4709,10 +4709,10 @@
         <v>0.590936018</v>
       </c>
       <c r="D124" t="n">
-        <v>23.52117604291561</v>
+        <v>23.57876202364988</v>
       </c>
       <c r="E124" t="n">
-        <v>6.152232133337318</v>
+        <v>6.15223213333732</v>
       </c>
       <c r="F124" t="n">
         <v>0.0006434559402011473</v>
@@ -4721,10 +4721,10 @@
         <v>1.364523076606728</v>
       </c>
       <c r="H124" t="n">
-        <v>23.57876202364987</v>
+        <v>17.75226826276409</v>
       </c>
       <c r="I124" t="n">
-        <v>0.3257383724515319</v>
+        <v>0.3257383724515306</v>
       </c>
       <c r="J124" t="n">
         <v>0.01995915477298129</v>
@@ -4746,7 +4746,7 @@
         <v>0.554336397</v>
       </c>
       <c r="D125" t="n">
-        <v>23.24380858655456</v>
+        <v>23.90661999573352</v>
       </c>
       <c r="E125" t="n">
         <v>4.735660116826642</v>
@@ -4758,10 +4758,10 @@
         <v>1.485615277236469</v>
       </c>
       <c r="H125" t="n">
-        <v>23.90661999573352</v>
+        <v>19.7282970910649</v>
       </c>
       <c r="I125" t="n">
-        <v>0.5573372121580258</v>
+        <v>0.5573372121580242</v>
       </c>
       <c r="J125" t="n">
         <v>0.008252140278192276</v>
@@ -4783,10 +4783,10 @@
         <v>0.481901397</v>
       </c>
       <c r="D126" t="n">
-        <v>17.80031520868662</v>
+        <v>15.52304868908039</v>
       </c>
       <c r="E126" t="n">
-        <v>0.4208253198561628</v>
+        <v>0.4208253198561652</v>
       </c>
       <c r="F126" t="n">
         <v>0.000324767235675073</v>
@@ -4795,10 +4795,10 @@
         <v>1.241271114558157</v>
       </c>
       <c r="H126" t="n">
-        <v>15.52304868908038</v>
+        <v>15.11004505196338</v>
       </c>
       <c r="I126" t="n">
-        <v>0.007821682739157731</v>
+        <v>0.007821682739157954</v>
       </c>
       <c r="J126" t="n">
         <v>0.001508581593900134</v>
@@ -4820,10 +4820,10 @@
         <v>1</v>
       </c>
       <c r="D127" t="n">
-        <v>21.31512992549159</v>
+        <v>22.63710681951976</v>
       </c>
       <c r="E127" t="n">
-        <v>5.62533273261054</v>
+        <v>5.625332732610541</v>
       </c>
       <c r="F127" t="n">
         <v>0.0006573497256845729</v>
@@ -4832,10 +4832,10 @@
         <v>1.484931628499323</v>
       </c>
       <c r="H127" t="n">
-        <v>22.63710681951976</v>
+        <v>18.21188787173196</v>
       </c>
       <c r="I127" t="n">
-        <v>1.200113784822744</v>
+        <v>1.200113784822742</v>
       </c>
       <c r="J127" t="n">
         <v>0.002843951336832681</v>

</xml_diff>